<commit_message>
some minor wording changes, change in leucas' location
</commit_message>
<xml_diff>
--- a/data (in excel format)/poets_cities.xlsx
+++ b/data (in excel format)/poets_cities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="poets" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="265">
   <si>
     <t>Melanippides</t>
   </si>
@@ -1274,7 +1274,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1284,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D132" sqref="D132"/>
+    <sheetView topLeftCell="A171" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D186" sqref="D186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6574,10 +6574,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B84"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B84"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:XFD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7097,193 +7097,185 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="3" t="s">
-        <v>38</v>
+        <v>234</v>
       </c>
       <c r="B61" s="6">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B62" s="6">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="3" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="B63" s="6">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B64" s="6">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B65" s="6">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B66" s="6">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="3" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="B67" s="6">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B68" s="6">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="3" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B69" s="6">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="3" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="B70" s="6">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B71" s="6">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B72" s="6">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="3" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="B73" s="6">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="3" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="B74" s="6">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="3" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="B75" s="6">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="3" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B76" s="6">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="3" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="B77" s="6">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B78" s="6">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B79" s="6">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="3" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
       <c r="B80" s="6">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="3" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="B81" s="6">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B82" s="6">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="3" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="B83" s="6">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B84" s="6">
         <v>85</v>
       </c>
     </row>

</xml_diff>